<commit_message>
Updated UI styling and charts
</commit_message>
<xml_diff>
--- a/Data/Data Analysis.xlsx
+++ b/Data/Data Analysis.xlsx
@@ -5147,8 +5147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK346"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="P321" workbookViewId="0">
+      <selection activeCell="X333" sqref="X333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>